<commit_message>
Corrected errors in the Laskowski database
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="1040">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="1034">
   <si>
     <t xml:space="preserve">Reduced Composition</t>
   </si>
@@ -1669,16 +1669,10 @@
     <t xml:space="preserve">Li7.8Al0.6Sc1.2Ti10.2P18.0O72.0</t>
   </si>
   <si>
-    <t xml:space="preserve">LiTi(PO4)3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li6.0Ti6.0P18.0O72.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li1.05Al0.05Ti0.95(PO4)3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li6.3Al0.3Ti5.7P18.0O72.0</t>
+    <t xml:space="preserve">Li1.05Al0.05Ti1.95(PO4)3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li6.3Al0.3Ti11.7P18.0O72.0</t>
   </si>
   <si>
     <t xml:space="preserve">Li1.1Al0.1Ti1.9(PO4)3</t>
@@ -1687,46 +1681,34 @@
     <t xml:space="preserve">Li6.6Al0.6Ti11.4P18.0O72.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Li1.4Al0.4Ti0.6(PO4)3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li8.4Al2.4Ti3.6P18.0O72.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li1.05Cr0.05Ti0.95(PO4)3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li6.3Cr0.3Ti5.7P18.0O72.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li1.1Cr0.1Ti0.9(PO4)3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li6.6Cr0.6Ti5.4P18.0O72.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li1.05Fe0.05Ti0.95(PO4)3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li6.3Fe0.3Ti5.7P18.0O72.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li1.1Fe0.1Ti0.9(PO4)3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li6.6Fe0.6Ti5.4P18.0O72.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li1.2Fe0.2Ti0.8(PO4)3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li7.2Fe1.2Ti4.8P18.0O72.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li1.3Fe0.3Ti0.7(PO4)3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li7.8Fe1.8Ti4.2P18.0O72.0</t>
+    <t xml:space="preserve">Li1.05Cr0.05Ti1.95(PO4)3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li6.3Cr0.3Ti11.7P18.0O72.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li1.1Cr0.1Ti1.9(PO4)3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li6.6Cr0.6Ti11.4P18.0O72.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li1.05Fe0.05Ti1.95(PO4)3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li6.3Fe0.3Ti11.7P18.0O72.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li1.1Fe0.1Ti1.9(PO4)3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li6.6Fe0.6Ti11.4P18.0O72.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li7.2Fe1.2Ti9.8P18.0O72.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li7.8Fe1.8Ti9.2P18.0O72.0</t>
   </si>
   <si>
     <t xml:space="preserve">Li1.3Al0.3Ge1.7(PO4)3</t>
@@ -3216,16 +3198,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3248,11 +3226,11 @@
   </sheetPr>
   <dimension ref="A1:K609"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A273" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C298" activeCellId="0" sqref="C298"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A413" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A441" activeCellId="0" sqref="A441"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.28"/>
@@ -3635,13 +3613,13 @@
       <c r="H11" s="0" t="n">
         <v>22.027</v>
       </c>
-      <c r="I11" s="2" t="n">
-        <v>90</v>
-      </c>
-      <c r="J11" s="2" t="n">
-        <v>90</v>
-      </c>
-      <c r="K11" s="2" t="n">
+      <c r="I11" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="K11" s="0" t="n">
         <v>120</v>
       </c>
     </row>
@@ -11551,7 +11529,7 @@
       <c r="J237" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="K237" s="2" t="n">
+      <c r="K237" s="0" t="n">
         <v>120</v>
       </c>
     </row>
@@ -13377,13 +13355,13 @@
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
-        <v>549</v>
+        <v>437</v>
       </c>
       <c r="B290" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C290" s="0" t="s">
-        <v>550</v>
+        <v>438</v>
       </c>
       <c r="D290" s="1" t="n">
         <v>6E-005</v>
@@ -13412,13 +13390,13 @@
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B291" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C291" s="0" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D291" s="0" t="n">
         <v>0.0011</v>
@@ -13447,13 +13425,13 @@
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B292" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C292" s="0" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D292" s="0" t="n">
         <v>0.00067</v>
@@ -13517,13 +13495,13 @@
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="s">
-        <v>555</v>
+        <v>481</v>
       </c>
       <c r="B294" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C294" s="0" t="s">
-        <v>556</v>
+        <v>482</v>
       </c>
       <c r="D294" s="0" t="n">
         <v>0.0033</v>
@@ -13552,13 +13530,13 @@
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B295" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C295" s="0" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D295" s="0" t="n">
         <v>0.00018</v>
@@ -13587,13 +13565,13 @@
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="B296" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C296" s="0" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="D296" s="0" t="n">
         <v>0.00026</v>
@@ -13692,13 +13670,13 @@
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B299" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C299" s="0" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D299" s="0" t="n">
         <v>0.00013</v>
@@ -13727,13 +13705,13 @@
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B300" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C300" s="0" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="D300" s="0" t="n">
         <v>0.00063</v>
@@ -13762,13 +13740,13 @@
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>565</v>
+        <v>501</v>
       </c>
       <c r="B301" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C301" s="0" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="D301" s="0" t="n">
         <v>0.0014</v>
@@ -13797,13 +13775,13 @@
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>567</v>
+        <v>503</v>
       </c>
       <c r="B302" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C302" s="0" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="D302" s="0" t="n">
         <v>0.0023</v>
@@ -13832,13 +13810,13 @@
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="B303" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C303" s="0" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="D303" s="1" t="n">
         <v>8.24E-005</v>
@@ -13867,13 +13845,13 @@
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="B304" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C304" s="0" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="D304" s="0" t="n">
         <v>0.000284</v>
@@ -13902,7 +13880,7 @@
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="B305" s="0" t="n">
         <v>6</v>
@@ -14147,13 +14125,13 @@
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="B312" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C312" s="0" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="D312" s="0" t="n">
         <v>0.0007</v>
@@ -14357,13 +14335,13 @@
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="B318" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C318" s="0" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="D318" s="0" t="n">
         <v>0.000522</v>
@@ -14462,13 +14440,13 @@
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="B321" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C321" s="0" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="D321" s="0" t="n">
         <v>0.000158</v>
@@ -14497,13 +14475,13 @@
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="B322" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C322" s="0" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="D322" s="1" t="n">
         <v>1E-005</v>
@@ -14532,13 +14510,13 @@
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="B323" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C323" s="0" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="D323" s="1" t="n">
         <v>5.6E-008</v>
@@ -14567,13 +14545,13 @@
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="B324" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C324" s="0" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="D324" s="1" t="n">
         <v>8.5E-008</v>
@@ -14602,13 +14580,13 @@
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="B325" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C325" s="0" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="D325" s="1" t="n">
         <v>3.2E-008</v>
@@ -14637,13 +14615,13 @@
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="0" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="B326" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C326" s="0" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="D326" s="1" t="n">
         <v>4E-006</v>
@@ -14707,13 +14685,13 @@
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="0" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="B328" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C328" s="0" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="D328" s="0" t="n">
         <v>0.000107</v>
@@ -14742,13 +14720,13 @@
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="0" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="B329" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C329" s="0" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="D329" s="1" t="n">
         <v>5.13E-005</v>
@@ -14777,13 +14755,13 @@
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="0" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="B330" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C330" s="0" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="D330" s="1" t="n">
         <v>5.88E-005</v>
@@ -14812,13 +14790,13 @@
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="0" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="B331" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C331" s="0" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="D331" s="1" t="n">
         <v>2.45E-005</v>
@@ -14847,13 +14825,13 @@
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="0" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="B332" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C332" s="0" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="D332" s="0" t="n">
         <v>0.000129</v>
@@ -14882,13 +14860,13 @@
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="0" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="B333" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C333" s="0" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="D333" s="1" t="n">
         <v>5.26E-007</v>
@@ -14917,13 +14895,13 @@
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="0" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="B334" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C334" s="0" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="D334" s="1" t="n">
         <v>5.4E-005</v>
@@ -14952,13 +14930,13 @@
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="B335" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C335" s="0" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="D335" s="0" t="n">
         <v>0.000142</v>
@@ -14987,13 +14965,13 @@
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="0" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="B336" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C336" s="0" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="D336" s="1" t="n">
         <v>3.56E-005</v>
@@ -15022,13 +15000,13 @@
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="0" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="B337" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C337" s="0" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="D337" s="1" t="n">
         <v>8.32E-005</v>
@@ -15057,13 +15035,13 @@
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="0" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="B338" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C338" s="0" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="D338" s="1" t="n">
         <v>3.19E-005</v>
@@ -15092,13 +15070,13 @@
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="0" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="B339" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C339" s="0" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="D339" s="0" t="n">
         <v>0.000142</v>
@@ -15127,13 +15105,13 @@
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="0" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="B340" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C340" s="0" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="D340" s="1" t="n">
         <v>2.06E-005</v>
@@ -15162,13 +15140,13 @@
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="0" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="B341" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C341" s="0" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="D341" s="1" t="n">
         <v>2.09E-005</v>
@@ -15232,13 +15210,13 @@
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="0" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="B343" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C343" s="0" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="D343" s="0" t="n">
         <v>0.00012</v>
@@ -15267,13 +15245,13 @@
     </row>
     <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="0" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="B344" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C344" s="0" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="D344" s="1" t="n">
         <v>7.3E-005</v>
@@ -15302,13 +15280,13 @@
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="0" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="B345" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C345" s="0" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="D345" s="1" t="n">
         <v>1.9E-005</v>
@@ -15337,13 +15315,13 @@
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="0" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="B346" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C346" s="0" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="D346" s="1" t="n">
         <v>2.9E-006</v>
@@ -15372,13 +15350,13 @@
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="0" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="B347" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C347" s="0" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="D347" s="1" t="n">
         <v>3.9E-005</v>
@@ -15442,13 +15420,13 @@
     </row>
     <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="0" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="B349" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C349" s="0" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="D349" s="0" t="n">
         <v>0.00014</v>
@@ -15477,13 +15455,13 @@
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="0" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B350" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C350" s="0" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D350" s="1" t="n">
         <v>3E-005</v>
@@ -15547,13 +15525,13 @@
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="0" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="B352" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C352" s="0" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="D352" s="1" t="n">
         <v>2.3E-005</v>
@@ -15617,13 +15595,13 @@
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="0" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B354" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C354" s="0" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D354" s="1" t="n">
         <v>5E-006</v>
@@ -15722,13 +15700,13 @@
     </row>
     <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="0" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="B357" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C357" s="0" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="D357" s="0" t="n">
         <v>0.00024</v>
@@ -15757,13 +15735,13 @@
     </row>
     <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="0" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="B358" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C358" s="0" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="D358" s="1" t="n">
         <v>6.5E-007</v>
@@ -15792,13 +15770,13 @@
     </row>
     <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="0" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="B359" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C359" s="0" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="D359" s="1" t="n">
         <v>6.5E-007</v>
@@ -15827,13 +15805,13 @@
     </row>
     <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="0" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="B360" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C360" s="0" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="D360" s="1" t="n">
         <v>3.57E-010</v>
@@ -15862,13 +15840,13 @@
     </row>
     <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="0" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="B361" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C361" s="0" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="D361" s="1" t="n">
         <v>3.17E-008</v>
@@ -15897,13 +15875,13 @@
     </row>
     <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="0" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="B362" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C362" s="0" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="D362" s="1" t="n">
         <v>1.37E-006</v>
@@ -15932,13 +15910,13 @@
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="0" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="B363" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C363" s="0" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D363" s="0" t="s">
         <v>25</v>
@@ -15967,13 +15945,13 @@
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="0" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="B364" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C364" s="0" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="D364" s="0" t="s">
         <v>25</v>
@@ -16002,13 +15980,13 @@
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="0" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="B365" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C365" s="0" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="D365" s="0" t="s">
         <v>25</v>
@@ -16037,13 +16015,13 @@
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="0" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="B366" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C366" s="0" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="D366" s="1" t="n">
         <v>1E-005</v>
@@ -16072,13 +16050,13 @@
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="0" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="B367" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C367" s="0" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="D367" s="0" t="s">
         <v>25</v>
@@ -16107,13 +16085,13 @@
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="0" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="B368" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C368" s="0" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="D368" s="0" t="n">
         <v>0.0005767</v>
@@ -16142,13 +16120,13 @@
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="0" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="B369" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C369" s="0" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="D369" s="0" t="s">
         <v>25</v>
@@ -16177,13 +16155,13 @@
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="0" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="B370" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C370" s="0" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="D370" s="0" t="n">
         <v>0.000703</v>
@@ -16212,13 +16190,13 @@
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="0" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="B371" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C371" s="0" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="D371" s="0" t="n">
         <v>0.0002085</v>
@@ -16247,13 +16225,13 @@
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="0" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="B372" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C372" s="0" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="D372" s="1" t="n">
         <v>6E-006</v>
@@ -16282,13 +16260,13 @@
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="0" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="B373" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C373" s="0" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="D373" s="1" t="n">
         <v>8E-006</v>
@@ -16317,13 +16295,13 @@
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="0" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="B374" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C374" s="0" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="D374" s="1" t="n">
         <v>7E-006</v>
@@ -16352,13 +16330,13 @@
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="0" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="B375" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C375" s="0" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="D375" s="1" t="n">
         <v>2.4E-005</v>
@@ -16387,13 +16365,13 @@
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="0" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="B376" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C376" s="0" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="D376" s="1" t="n">
         <v>1.06E-005</v>
@@ -16422,13 +16400,13 @@
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="0" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="B377" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C377" s="0" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="D377" s="1" t="n">
         <v>1.36E-008</v>
@@ -16457,13 +16435,13 @@
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="0" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="B378" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C378" s="0" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="D378" s="1" t="n">
         <v>1.8E-005</v>
@@ -16492,13 +16470,13 @@
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="0" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="B379" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C379" s="0" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="D379" s="1" t="n">
         <v>4.5E-005</v>
@@ -16527,13 +16505,13 @@
     </row>
     <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="0" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
       <c r="B380" s="0" t="n">
         <v>16</v>
       </c>
       <c r="C380" s="0" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="D380" s="1" t="n">
         <v>5E-008</v>
@@ -16562,13 +16540,13 @@
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="0" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="B381" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C381" s="0" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
       <c r="D381" s="0" t="s">
         <v>25</v>
@@ -16597,13 +16575,13 @@
     </row>
     <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="0" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="B382" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C382" s="0" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="D382" s="0" t="s">
         <v>25</v>
@@ -16632,13 +16610,13 @@
     </row>
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="0" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="B383" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C383" s="0" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
       <c r="D383" s="0" t="s">
         <v>25</v>
@@ -16667,13 +16645,13 @@
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="0" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
       <c r="B384" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C384" s="0" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
       <c r="D384" s="0" t="s">
         <v>25</v>
@@ -16702,13 +16680,13 @@
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="0" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="B385" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C385" s="0" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="D385" s="1" t="n">
         <v>6.56E-010</v>
@@ -16737,13 +16715,13 @@
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="0" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="B386" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C386" s="0" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
       <c r="D386" s="1" t="n">
         <v>1.53E-011</v>
@@ -16772,13 +16750,13 @@
     </row>
     <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="0" t="s">
-        <v>685</v>
+        <v>679</v>
       </c>
       <c r="B387" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C387" s="0" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="D387" s="1" t="n">
         <v>1E-009</v>
@@ -16807,13 +16785,13 @@
     </row>
     <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="0" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
       <c r="B388" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C388" s="0" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
       <c r="D388" s="1" t="n">
         <v>6.95E-006</v>
@@ -16842,13 +16820,13 @@
     </row>
     <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="0" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
       <c r="B389" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C389" s="0" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="D389" s="0" t="n">
         <v>0.00186</v>
@@ -16877,13 +16855,13 @@
     </row>
     <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="0" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="B390" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C390" s="0" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
       <c r="D390" s="0" t="n">
         <v>0.00205</v>
@@ -16912,13 +16890,13 @@
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="0" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="B391" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C391" s="0" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
       <c r="D391" s="0" t="n">
         <v>0.00333</v>
@@ -16947,13 +16925,13 @@
     </row>
     <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="0" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="B392" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C392" s="0" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="D392" s="0" t="n">
         <v>0.00115</v>
@@ -16982,13 +16960,13 @@
     </row>
     <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="0" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="B393" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C393" s="0" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="D393" s="1" t="n">
         <v>2.62E-005</v>
@@ -17017,13 +16995,13 @@
     </row>
     <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="0" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="B394" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C394" s="0" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
       <c r="D394" s="1" t="n">
         <v>1.3E-006</v>
@@ -17052,13 +17030,13 @@
     </row>
     <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="0" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
       <c r="B395" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C395" s="0" t="s">
-        <v>702</v>
+        <v>696</v>
       </c>
       <c r="D395" s="0" t="n">
         <v>0.00226</v>
@@ -17087,13 +17065,13 @@
     </row>
     <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="0" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
       <c r="B396" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C396" s="0" t="s">
-        <v>704</v>
+        <v>698</v>
       </c>
       <c r="D396" s="0" t="n">
         <v>0.000112</v>
@@ -17122,13 +17100,13 @@
     </row>
     <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="0" t="s">
-        <v>705</v>
+        <v>699</v>
       </c>
       <c r="B397" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C397" s="0" t="s">
-        <v>706</v>
+        <v>700</v>
       </c>
       <c r="D397" s="1" t="n">
         <v>4.72E-006</v>
@@ -17157,13 +17135,13 @@
     </row>
     <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="0" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="B398" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C398" s="0" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="D398" s="0" t="n">
         <v>0.000701</v>
@@ -17192,13 +17170,13 @@
     </row>
     <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="0" t="s">
-        <v>707</v>
+        <v>701</v>
       </c>
       <c r="B399" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C399" s="0" t="s">
-        <v>708</v>
+        <v>702</v>
       </c>
       <c r="D399" s="0" t="n">
         <v>0.000878</v>
@@ -17227,13 +17205,13 @@
     </row>
     <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="0" t="s">
-        <v>709</v>
+        <v>703</v>
       </c>
       <c r="B400" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C400" s="0" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
       <c r="D400" s="0" t="n">
         <v>0.000437</v>
@@ -17262,13 +17240,13 @@
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="s">
-        <v>711</v>
+        <v>705</v>
       </c>
       <c r="B401" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C401" s="0" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
       <c r="D401" s="0" t="n">
         <v>0.000873</v>
@@ -17297,13 +17275,13 @@
     </row>
     <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="0" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
       <c r="B402" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C402" s="0" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="D402" s="0" t="n">
         <v>0.000799</v>
@@ -17332,13 +17310,13 @@
     </row>
     <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="0" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
       <c r="B403" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C403" s="0" t="s">
-        <v>716</v>
+        <v>710</v>
       </c>
       <c r="D403" s="0" t="n">
         <v>0.000902</v>
@@ -17367,13 +17345,13 @@
     </row>
     <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="0" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
       <c r="B404" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C404" s="0" t="s">
-        <v>718</v>
+        <v>712</v>
       </c>
       <c r="D404" s="0" t="n">
         <v>0.000931</v>
@@ -17402,13 +17380,13 @@
     </row>
     <row r="405" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="0" t="s">
-        <v>719</v>
+        <v>713</v>
       </c>
       <c r="B405" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C405" s="0" t="s">
-        <v>720</v>
+        <v>714</v>
       </c>
       <c r="D405" s="0" t="n">
         <v>0.00169</v>
@@ -17437,13 +17415,13 @@
     </row>
     <row r="406" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="0" t="s">
-        <v>721</v>
+        <v>715</v>
       </c>
       <c r="B406" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C406" s="0" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="D406" s="0" t="n">
         <v>0.00108</v>
@@ -17472,13 +17450,13 @@
     </row>
     <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="0" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
       <c r="B407" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C407" s="0" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="D407" s="0" t="n">
         <v>0.00141</v>
@@ -17507,13 +17485,13 @@
     </row>
     <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="0" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
       <c r="B408" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C408" s="0" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="D408" s="0" t="n">
         <v>0.00165</v>
@@ -17542,13 +17520,13 @@
     </row>
     <row r="409" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="0" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="B409" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C409" s="0" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="D409" s="0" t="n">
         <v>0.00234</v>
@@ -17577,13 +17555,13 @@
     </row>
     <row r="410" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="0" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="B410" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C410" s="0" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="D410" s="0" t="n">
         <v>0.00219</v>
@@ -17612,13 +17590,13 @@
     </row>
     <row r="411" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="0" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="B411" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C411" s="0" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="D411" s="0" t="n">
         <v>0.00011</v>
@@ -17647,13 +17625,13 @@
     </row>
     <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="0" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="B412" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C412" s="0" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
       <c r="D412" s="0" t="n">
         <v>0.0013</v>
@@ -17682,13 +17660,13 @@
     </row>
     <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="0" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="B413" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C413" s="0" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="D413" s="0" t="n">
         <v>0.00277</v>
@@ -17717,13 +17695,13 @@
     </row>
     <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="0" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="B414" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C414" s="0" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="D414" s="0" t="n">
         <v>0.0032</v>
@@ -17752,13 +17730,13 @@
     </row>
     <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="0" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="B415" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C415" s="0" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="D415" s="0" t="n">
         <v>0.00392</v>
@@ -17787,13 +17765,13 @@
     </row>
     <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="0" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
       <c r="B416" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C416" s="0" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="D416" s="0" t="n">
         <v>0.00362</v>
@@ -17822,13 +17800,13 @@
     </row>
     <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="0" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="B417" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C417" s="0" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="D417" s="0" t="n">
         <v>0.00364</v>
@@ -17857,13 +17835,13 @@
     </row>
     <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="0" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="B418" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C418" s="0" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="D418" s="0" t="n">
         <v>0.00268</v>
@@ -17892,13 +17870,13 @@
     </row>
     <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="0" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
       <c r="B419" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C419" s="0" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="D419" s="0" t="n">
         <v>0.00278</v>
@@ -17927,13 +17905,13 @@
     </row>
     <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="0" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
       <c r="B420" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C420" s="0" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="D420" s="0" t="n">
         <v>0.00301</v>
@@ -17962,13 +17940,13 @@
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="0" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="B421" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C421" s="0" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="D421" s="0" t="n">
         <v>0.00348</v>
@@ -17997,13 +17975,13 @@
     </row>
     <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="0" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
       <c r="B422" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C422" s="0" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="D422" s="0" t="n">
         <v>0.00382</v>
@@ -18032,13 +18010,13 @@
     </row>
     <row r="423" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="0" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="B423" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C423" s="0" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="D423" s="0" t="n">
         <v>0.00361</v>
@@ -18067,13 +18045,13 @@
     </row>
     <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="0" t="s">
-        <v>685</v>
+        <v>679</v>
       </c>
       <c r="B424" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C424" s="0" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="D424" s="1" t="n">
         <v>5.54E-010</v>
@@ -18102,13 +18080,13 @@
     </row>
     <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="0" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="B425" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C425" s="0" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="D425" s="1" t="n">
         <v>3.2E-005</v>
@@ -18137,13 +18115,13 @@
     </row>
     <row r="426" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="0" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="B426" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C426" s="0" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
       <c r="D426" s="1" t="n">
         <v>3.3E-005</v>
@@ -18172,13 +18150,13 @@
     </row>
     <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="B427" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C427" s="0" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
       <c r="D427" s="0" t="n">
         <v>0.00022</v>
@@ -18207,13 +18185,13 @@
     </row>
     <row r="428" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="B428" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C428" s="0" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
       <c r="D428" s="1" t="n">
         <v>1.74E-006</v>
@@ -18242,13 +18220,13 @@
     </row>
     <row r="429" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="0" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="B429" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C429" s="0" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="D429" s="1" t="n">
         <v>8.86E-006</v>
@@ -18277,13 +18255,13 @@
     </row>
     <row r="430" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="0" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="B430" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C430" s="0" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="D430" s="1" t="n">
         <v>3.93E-005</v>
@@ -18312,13 +18290,13 @@
     </row>
     <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="0" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="B431" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C431" s="0" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
       <c r="D431" s="1" t="n">
         <v>3.19E-005</v>
@@ -18347,13 +18325,13 @@
     </row>
     <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="0" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="B432" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C432" s="0" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="D432" s="0" t="n">
         <v>0.00015</v>
@@ -18382,13 +18360,13 @@
     </row>
     <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="0" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="B433" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C433" s="0" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="D433" s="0" t="n">
         <v>0.00065</v>
@@ -18417,13 +18395,13 @@
     </row>
     <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="0" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="B434" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C434" s="0" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="D434" s="0" t="n">
         <v>0.0015</v>
@@ -18452,13 +18430,13 @@
     </row>
     <row r="435" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="0" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="B435" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C435" s="0" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="D435" s="0" t="n">
         <v>0.00186</v>
@@ -18487,13 +18465,13 @@
     </row>
     <row r="436" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="0" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="B436" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C436" s="0" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
       <c r="D436" s="0" t="n">
         <v>0.00521</v>
@@ -18522,13 +18500,13 @@
     </row>
     <row r="437" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="0" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
       <c r="B437" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C437" s="0" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="D437" s="0" t="n">
         <v>0.00554</v>
@@ -18557,13 +18535,13 @@
     </row>
     <row r="438" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="0" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="B438" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C438" s="0" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="D438" s="0" t="n">
         <v>0.00258</v>
@@ -18592,13 +18570,13 @@
     </row>
     <row r="439" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="0" t="s">
-        <v>685</v>
+        <v>679</v>
       </c>
       <c r="B439" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C439" s="0" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="D439" s="1" t="n">
         <v>1E-009</v>
@@ -18627,13 +18605,13 @@
     </row>
     <row r="440" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="0" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="B440" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C440" s="0" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
       <c r="D440" s="1" t="n">
         <v>4.6E-007</v>
@@ -18662,13 +18640,13 @@
     </row>
     <row r="441" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="0" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
       <c r="B441" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C441" s="0" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="D441" s="0" t="n">
         <v>0.0018</v>
@@ -18697,13 +18675,13 @@
     </row>
     <row r="442" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="0" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="B442" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C442" s="0" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
       <c r="D442" s="0" t="n">
         <v>0.000103</v>
@@ -18732,13 +18710,13 @@
     </row>
     <row r="443" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="0" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="B443" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C443" s="0" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="D443" s="1" t="n">
         <v>8.6E-005</v>
@@ -18767,13 +18745,13 @@
     </row>
     <row r="444" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="0" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
       <c r="B444" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C444" s="0" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
       <c r="D444" s="1" t="n">
         <v>2.4E-005</v>
@@ -18802,13 +18780,13 @@
     </row>
     <row r="445" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="0" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="B445" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C445" s="0" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
       <c r="D445" s="0" t="n">
         <v>0.000935</v>
@@ -18837,13 +18815,13 @@
     </row>
     <row r="446" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="0" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
       <c r="B446" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C446" s="0" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="D446" s="0" t="n">
         <v>0.00138</v>
@@ -18872,13 +18850,13 @@
     </row>
     <row r="447" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="0" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="B447" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C447" s="0" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="D447" s="0" t="n">
         <v>0.025</v>
@@ -18907,13 +18885,13 @@
     </row>
     <row r="448" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="0" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="B448" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C448" s="0" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
       <c r="D448" s="0" t="n">
         <v>0.00026</v>
@@ -18942,13 +18920,13 @@
     </row>
     <row r="449" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="0" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="B449" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C449" s="0" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="D449" s="1" t="n">
         <v>3.86E-005</v>
@@ -18977,13 +18955,13 @@
     </row>
     <row r="450" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="0" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
       <c r="B450" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C450" s="0" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
       <c r="D450" s="1" t="n">
         <v>1.2E-006</v>
@@ -19012,13 +18990,13 @@
     </row>
     <row r="451" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="0" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="B451" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C451" s="0" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="D451" s="0" t="n">
         <v>0.00151</v>
@@ -19047,13 +19025,13 @@
     </row>
     <row r="452" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="0" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
       <c r="B452" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C452" s="0" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
       <c r="D452" s="0" t="n">
         <v>0.000568</v>
@@ -19082,13 +19060,13 @@
     </row>
     <row r="453" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="0" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
       <c r="B453" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C453" s="0" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
       <c r="D453" s="0" t="n">
         <v>0.000161</v>
@@ -19117,13 +19095,13 @@
     </row>
     <row r="454" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="0" t="s">
-        <v>797</v>
+        <v>791</v>
       </c>
       <c r="B454" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C454" s="0" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
       <c r="D454" s="1" t="n">
         <v>1.04E-007</v>
@@ -19152,13 +19130,13 @@
     </row>
     <row r="455" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="0" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
       <c r="B455" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C455" s="0" t="s">
-        <v>800</v>
+        <v>794</v>
       </c>
       <c r="D455" s="0" t="n">
         <v>0.00038</v>
@@ -19187,13 +19165,13 @@
     </row>
     <row r="456" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="0" t="s">
-        <v>801</v>
+        <v>795</v>
       </c>
       <c r="B456" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C456" s="0" t="s">
-        <v>802</v>
+        <v>796</v>
       </c>
       <c r="D456" s="1" t="n">
         <v>1.13E-005</v>
@@ -19222,13 +19200,13 @@
     </row>
     <row r="457" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="0" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
       <c r="B457" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C457" s="0" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
       <c r="D457" s="1" t="n">
         <v>1.37E-005</v>
@@ -19257,13 +19235,13 @@
     </row>
     <row r="458" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="0" t="s">
-        <v>805</v>
+        <v>799</v>
       </c>
       <c r="B458" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C458" s="0" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="D458" s="1" t="n">
         <v>5.3E-005</v>
@@ -19292,13 +19270,13 @@
     </row>
     <row r="459" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="0" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
       <c r="B459" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C459" s="0" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
       <c r="D459" s="1" t="n">
         <v>7.64E-005</v>
@@ -19327,13 +19305,13 @@
     </row>
     <row r="460" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="0" t="s">
-        <v>809</v>
+        <v>803</v>
       </c>
       <c r="B460" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C460" s="0" t="s">
-        <v>810</v>
+        <v>804</v>
       </c>
       <c r="D460" s="1" t="n">
         <v>6.04E-005</v>
@@ -19362,13 +19340,13 @@
     </row>
     <row r="461" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="0" t="s">
-        <v>811</v>
+        <v>805</v>
       </c>
       <c r="B461" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C461" s="0" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="D461" s="1" t="n">
         <v>1.92E-005</v>
@@ -19403,7 +19381,7 @@
         <v>1</v>
       </c>
       <c r="C462" s="0" t="s">
-        <v>813</v>
+        <v>807</v>
       </c>
       <c r="D462" s="0" t="n">
         <v>0.000832</v>
@@ -19438,7 +19416,7 @@
         <v>1</v>
       </c>
       <c r="C463" s="0" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="D463" s="0" t="n">
         <v>0.0013</v>
@@ -19473,7 +19451,7 @@
         <v>1</v>
       </c>
       <c r="C464" s="0" t="s">
-        <v>815</v>
+        <v>809</v>
       </c>
       <c r="D464" s="0" t="n">
         <v>0.00154</v>
@@ -19508,7 +19486,7 @@
         <v>1</v>
       </c>
       <c r="C465" s="0" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
       <c r="D465" s="0" t="n">
         <v>0.00125</v>
@@ -19543,7 +19521,7 @@
         <v>1</v>
       </c>
       <c r="C466" s="0" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
       <c r="D466" s="0" t="n">
         <v>0.000785</v>
@@ -19572,13 +19550,13 @@
     </row>
     <row r="467" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="0" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="B467" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C467" s="0" t="s">
-        <v>819</v>
+        <v>813</v>
       </c>
       <c r="D467" s="1" t="n">
         <v>7E-005</v>
@@ -19607,13 +19585,13 @@
     </row>
     <row r="468" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="0" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="B468" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C468" s="0" t="s">
-        <v>821</v>
+        <v>815</v>
       </c>
       <c r="D468" s="1" t="n">
         <v>1.1E-006</v>
@@ -19642,13 +19620,13 @@
     </row>
     <row r="469" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="0" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="B469" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C469" s="0" t="s">
-        <v>821</v>
+        <v>815</v>
       </c>
       <c r="D469" s="1" t="n">
         <v>1.06E-006</v>
@@ -19677,13 +19655,13 @@
     </row>
     <row r="470" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="0" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="B470" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C470" s="0" t="s">
-        <v>823</v>
+        <v>817</v>
       </c>
       <c r="D470" s="1" t="n">
         <v>2.61E-005</v>
@@ -19712,13 +19690,13 @@
     </row>
     <row r="471" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="0" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="B471" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C471" s="0" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
       <c r="D471" s="1" t="n">
         <v>6E-005</v>
@@ -19747,13 +19725,13 @@
     </row>
     <row r="472" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="0" t="s">
-        <v>826</v>
+        <v>820</v>
       </c>
       <c r="B472" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C472" s="0" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="D472" s="0" t="n">
         <v>0.0001</v>
@@ -19782,13 +19760,13 @@
     </row>
     <row r="473" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="0" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="B473" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C473" s="0" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
       <c r="D473" s="0" t="n">
         <v>0.000108</v>
@@ -19817,13 +19795,13 @@
     </row>
     <row r="474" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="0" t="s">
-        <v>830</v>
+        <v>824</v>
       </c>
       <c r="B474" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C474" s="0" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="D474" s="1" t="n">
         <v>1E-008</v>
@@ -19852,13 +19830,13 @@
     </row>
     <row r="475" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="0" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="B475" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C475" s="0" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
       <c r="D475" s="1" t="n">
         <v>6.03E-008</v>
@@ -19887,13 +19865,13 @@
     </row>
     <row r="476" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="0" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
       <c r="B476" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C476" s="0" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="D476" s="1" t="n">
         <v>1.73E-008</v>
@@ -19922,13 +19900,13 @@
     </row>
     <row r="477" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="0" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="B477" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C477" s="0" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="D477" s="1" t="n">
         <v>4.24E-009</v>
@@ -19957,13 +19935,13 @@
     </row>
     <row r="478" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="0" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
       <c r="B478" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C478" s="0" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="D478" s="1" t="n">
         <v>1.51E-009</v>
@@ -19992,13 +19970,13 @@
     </row>
     <row r="479" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="0" t="s">
-        <v>840</v>
+        <v>834</v>
       </c>
       <c r="B479" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C479" s="0" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
       <c r="D479" s="1" t="n">
         <v>4.79E-006</v>
@@ -20027,13 +20005,13 @@
     </row>
     <row r="480" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="0" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="B480" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C480" s="0" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="D480" s="1" t="n">
         <v>6.24E-007</v>
@@ -20062,13 +20040,13 @@
     </row>
     <row r="481" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="0" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="B481" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C481" s="0" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="D481" s="1" t="n">
         <v>2.37E-007</v>
@@ -20097,13 +20075,13 @@
     </row>
     <row r="482" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="0" t="s">
-        <v>846</v>
+        <v>840</v>
       </c>
       <c r="B482" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C482" s="0" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="D482" s="1" t="n">
         <v>9.9E-008</v>
@@ -20132,13 +20110,13 @@
     </row>
     <row r="483" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="0" t="s">
-        <v>848</v>
+        <v>842</v>
       </c>
       <c r="B483" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C483" s="0" t="s">
-        <v>849</v>
+        <v>843</v>
       </c>
       <c r="D483" s="1" t="n">
         <v>5.8E-007</v>
@@ -20167,13 +20145,13 @@
     </row>
     <row r="484" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="0" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="B484" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C484" s="0" t="s">
-        <v>851</v>
+        <v>845</v>
       </c>
       <c r="D484" s="0" t="s">
         <v>25</v>
@@ -20202,13 +20180,13 @@
     </row>
     <row r="485" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="0" t="s">
-        <v>852</v>
+        <v>846</v>
       </c>
       <c r="B485" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C485" s="0" t="s">
-        <v>853</v>
+        <v>847</v>
       </c>
       <c r="D485" s="0" t="s">
         <v>25</v>
@@ -20237,13 +20215,13 @@
     </row>
     <row r="486" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="0" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="B486" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C486" s="0" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="D486" s="0" t="s">
         <v>25</v>
@@ -20272,13 +20250,13 @@
     </row>
     <row r="487" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="0" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
       <c r="B487" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C487" s="0" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="D487" s="0" t="s">
         <v>25</v>
@@ -20307,13 +20285,13 @@
     </row>
     <row r="488" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="0" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="B488" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C488" s="0" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
       <c r="D488" s="0" t="s">
         <v>25</v>
@@ -20342,13 +20320,13 @@
     </row>
     <row r="489" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="0" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="B489" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C489" s="0" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="D489" s="0" t="s">
         <v>25</v>
@@ -20412,13 +20390,13 @@
     </row>
     <row r="491" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="0" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="B491" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C491" s="0" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="D491" s="1" t="n">
         <v>6.21E-007</v>
@@ -20447,13 +20425,13 @@
     </row>
     <row r="492" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="0" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="B492" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C492" s="0" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
       <c r="D492" s="1" t="n">
         <v>4.2E-006</v>
@@ -20482,13 +20460,13 @@
     </row>
     <row r="493" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="0" t="s">
-        <v>866</v>
+        <v>860</v>
       </c>
       <c r="B493" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C493" s="0" t="s">
-        <v>867</v>
+        <v>861</v>
       </c>
       <c r="D493" s="1" t="n">
         <v>1.6E-006</v>
@@ -20517,13 +20495,13 @@
     </row>
     <row r="494" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="0" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="B494" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C494" s="0" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
       <c r="D494" s="1" t="n">
         <v>7.41E-006</v>
@@ -20552,13 +20530,13 @@
     </row>
     <row r="495" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="0" t="s">
-        <v>870</v>
+        <v>864</v>
       </c>
       <c r="B495" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C495" s="0" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="D495" s="1" t="n">
         <v>1.41E-005</v>
@@ -20587,13 +20565,13 @@
     </row>
     <row r="496" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="0" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="B496" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C496" s="0" t="s">
-        <v>873</v>
+        <v>867</v>
       </c>
       <c r="D496" s="1" t="n">
         <v>4.99E-005</v>
@@ -20622,13 +20600,13 @@
     </row>
     <row r="497" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="0" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
       <c r="B497" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C497" s="0" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="D497" s="1" t="n">
         <v>3.08E-005</v>
@@ -20657,13 +20635,13 @@
     </row>
     <row r="498" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="0" t="s">
-        <v>876</v>
+        <v>870</v>
       </c>
       <c r="B498" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C498" s="0" t="s">
-        <v>877</v>
+        <v>871</v>
       </c>
       <c r="D498" s="1" t="n">
         <v>1.18E-005</v>
@@ -20692,13 +20670,13 @@
     </row>
     <row r="499" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="0" t="s">
-        <v>878</v>
+        <v>872</v>
       </c>
       <c r="B499" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C499" s="0" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
       <c r="D499" s="1" t="n">
         <v>2.85E-006</v>
@@ -20727,13 +20705,13 @@
     </row>
     <row r="500" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="0" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="B500" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C500" s="0" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="D500" s="1" t="n">
         <v>6.61E-006</v>
@@ -20762,13 +20740,13 @@
     </row>
     <row r="501" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="0" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="B501" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C501" s="0" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="D501" s="1" t="n">
         <v>2.95E-005</v>
@@ -20797,13 +20775,13 @@
     </row>
     <row r="502" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="0" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="B502" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C502" s="0" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="D502" s="0" t="n">
         <v>0.00034</v>
@@ -20832,13 +20810,13 @@
     </row>
     <row r="503" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="0" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="B503" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C503" s="0" t="s">
-        <v>887</v>
+        <v>881</v>
       </c>
       <c r="D503" s="0" t="n">
         <v>0.00081</v>
@@ -20867,13 +20845,13 @@
     </row>
     <row r="504" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="0" t="s">
-        <v>888</v>
+        <v>882</v>
       </c>
       <c r="B504" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C504" s="0" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="D504" s="0" t="n">
         <v>0.00035</v>
@@ -20902,13 +20880,13 @@
     </row>
     <row r="505" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="0" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
       <c r="B505" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C505" s="0" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="D505" s="0" t="n">
         <v>0.00028</v>
@@ -20937,13 +20915,13 @@
     </row>
     <row r="506" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="0" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="B506" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C506" s="0" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="D506" s="0" t="n">
         <v>0.00073</v>
@@ -20972,13 +20950,13 @@
     </row>
     <row r="507" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="0" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="B507" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C507" s="0" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="D507" s="0" t="n">
         <v>0.00092</v>
@@ -21007,13 +20985,13 @@
     </row>
     <row r="508" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="0" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="B508" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C508" s="0" t="s">
-        <v>897</v>
+        <v>891</v>
       </c>
       <c r="D508" s="0" t="n">
         <v>0.001</v>
@@ -21042,13 +21020,13 @@
     </row>
     <row r="509" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="0" t="s">
-        <v>898</v>
+        <v>892</v>
       </c>
       <c r="B509" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C509" s="0" t="s">
-        <v>899</v>
+        <v>893</v>
       </c>
       <c r="D509" s="0" t="n">
         <v>0.00032</v>
@@ -21077,13 +21055,13 @@
     </row>
     <row r="510" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="0" t="s">
-        <v>900</v>
+        <v>894</v>
       </c>
       <c r="B510" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C510" s="0" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="D510" s="0" t="n">
         <v>0.00016</v>
@@ -21112,13 +21090,13 @@
     </row>
     <row r="511" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="0" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
       <c r="B511" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C511" s="0" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="D511" s="0" t="n">
         <v>0.00073</v>
@@ -21147,13 +21125,13 @@
     </row>
     <row r="512" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="0" t="s">
-        <v>902</v>
+        <v>896</v>
       </c>
       <c r="B512" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C512" s="0" t="s">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="D512" s="0" t="n">
         <v>0.00063</v>
@@ -21182,13 +21160,13 @@
     </row>
     <row r="513" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="0" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="B513" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C513" s="0" t="s">
-        <v>905</v>
+        <v>899</v>
       </c>
       <c r="D513" s="0" t="n">
         <v>0.00046</v>
@@ -21217,13 +21195,13 @@
     </row>
     <row r="514" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="0" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="B514" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C514" s="0" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="D514" s="0" t="n">
         <v>0.00047</v>
@@ -21252,13 +21230,13 @@
     </row>
     <row r="515" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A515" s="0" t="s">
-        <v>906</v>
+        <v>900</v>
       </c>
       <c r="B515" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C515" s="0" t="s">
-        <v>907</v>
+        <v>901</v>
       </c>
       <c r="D515" s="0" t="n">
         <v>0.0004</v>
@@ -21287,13 +21265,13 @@
     </row>
     <row r="516" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A516" s="0" t="s">
-        <v>900</v>
+        <v>894</v>
       </c>
       <c r="B516" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C516" s="0" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="D516" s="0" t="n">
         <v>0.00035</v>
@@ -21322,13 +21300,13 @@
     </row>
     <row r="517" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A517" s="0" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="B517" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C517" s="0" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="D517" s="1" t="n">
         <v>3.4E-005</v>
@@ -21357,13 +21335,13 @@
     </row>
     <row r="518" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A518" s="0" t="s">
-        <v>908</v>
+        <v>902</v>
       </c>
       <c r="B518" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C518" s="0" t="s">
-        <v>909</v>
+        <v>903</v>
       </c>
       <c r="D518" s="0" t="n">
         <v>0.00069</v>
@@ -21392,13 +21370,13 @@
     </row>
     <row r="519" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A519" s="0" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="B519" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C519" s="0" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="D519" s="0" t="n">
         <v>0.00028</v>
@@ -21427,13 +21405,13 @@
     </row>
     <row r="520" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="0" t="s">
-        <v>910</v>
+        <v>904</v>
       </c>
       <c r="B520" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C520" s="0" t="s">
-        <v>911</v>
+        <v>905</v>
       </c>
       <c r="D520" s="0" t="n">
         <v>0.00128</v>
@@ -21462,13 +21440,13 @@
     </row>
     <row r="521" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="0" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="B521" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C521" s="0" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="D521" s="0" t="n">
         <v>0.00049</v>
@@ -21497,13 +21475,13 @@
     </row>
     <row r="522" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="0" t="s">
-        <v>914</v>
+        <v>908</v>
       </c>
       <c r="B522" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C522" s="0" t="s">
-        <v>915</v>
+        <v>909</v>
       </c>
       <c r="D522" s="1" t="n">
         <v>8E-005</v>
@@ -21532,13 +21510,13 @@
     </row>
     <row r="523" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="0" t="s">
-        <v>916</v>
+        <v>910</v>
       </c>
       <c r="B523" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C523" s="0" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="D523" s="0" t="n">
         <v>0.000311</v>
@@ -21567,13 +21545,13 @@
     </row>
     <row r="524" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A524" s="0" t="s">
-        <v>918</v>
+        <v>912</v>
       </c>
       <c r="B524" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C524" s="0" t="s">
-        <v>919</v>
+        <v>913</v>
       </c>
       <c r="D524" s="0" t="n">
         <v>0.000369</v>
@@ -21602,13 +21580,13 @@
     </row>
     <row r="525" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A525" s="0" t="s">
-        <v>920</v>
+        <v>914</v>
       </c>
       <c r="B525" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C525" s="0" t="s">
-        <v>921</v>
+        <v>915</v>
       </c>
       <c r="D525" s="0" t="n">
         <v>0.00034</v>
@@ -21637,13 +21615,13 @@
     </row>
     <row r="526" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A526" s="0" t="s">
-        <v>922</v>
+        <v>916</v>
       </c>
       <c r="B526" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C526" s="0" t="s">
-        <v>923</v>
+        <v>917</v>
       </c>
       <c r="D526" s="0" t="n">
         <v>0.000333</v>
@@ -21672,13 +21650,13 @@
     </row>
     <row r="527" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A527" s="0" t="s">
-        <v>924</v>
+        <v>918</v>
       </c>
       <c r="B527" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C527" s="0" t="s">
-        <v>925</v>
+        <v>919</v>
       </c>
       <c r="D527" s="0" t="n">
         <v>0.00033</v>
@@ -21707,13 +21685,13 @@
     </row>
     <row r="528" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A528" s="0" t="s">
-        <v>926</v>
+        <v>920</v>
       </c>
       <c r="B528" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C528" s="0" t="s">
-        <v>927</v>
+        <v>921</v>
       </c>
       <c r="D528" s="0" t="n">
         <v>0.00102</v>
@@ -21742,13 +21720,13 @@
     </row>
     <row r="529" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A529" s="0" t="s">
-        <v>928</v>
+        <v>922</v>
       </c>
       <c r="B529" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C529" s="0" t="s">
-        <v>929</v>
+        <v>923</v>
       </c>
       <c r="D529" s="1" t="n">
         <v>1.9E-005</v>
@@ -21777,13 +21755,13 @@
     </row>
     <row r="530" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="0" t="s">
-        <v>930</v>
+        <v>924</v>
       </c>
       <c r="B530" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C530" s="0" t="s">
-        <v>931</v>
+        <v>925</v>
       </c>
       <c r="D530" s="1" t="n">
         <v>2E-005</v>
@@ -21812,13 +21790,13 @@
     </row>
     <row r="531" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="B531" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C531" s="0" t="s">
-        <v>933</v>
+        <v>927</v>
       </c>
       <c r="D531" s="1" t="n">
         <v>1.3E-007</v>
@@ -21847,13 +21825,13 @@
     </row>
     <row r="532" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="0" t="s">
-        <v>934</v>
+        <v>928</v>
       </c>
       <c r="B532" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C532" s="0" t="s">
-        <v>935</v>
+        <v>929</v>
       </c>
       <c r="D532" s="1" t="n">
         <v>8.7E-009</v>
@@ -21882,13 +21860,13 @@
     </row>
     <row r="533" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>936</v>
+        <v>930</v>
       </c>
       <c r="B533" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C533" s="0" t="s">
-        <v>937</v>
+        <v>931</v>
       </c>
       <c r="D533" s="1" t="n">
         <v>7.8E-006</v>
@@ -21917,13 +21895,13 @@
     </row>
     <row r="534" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>938</v>
+        <v>932</v>
       </c>
       <c r="B534" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C534" s="0" t="s">
-        <v>939</v>
+        <v>933</v>
       </c>
       <c r="D534" s="1" t="n">
         <v>6.3E-006</v>
@@ -21952,13 +21930,13 @@
     </row>
     <row r="535" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="0" t="s">
-        <v>940</v>
+        <v>934</v>
       </c>
       <c r="B535" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C535" s="0" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="D535" s="1" t="n">
         <v>1.33E-006</v>
@@ -21987,13 +21965,13 @@
     </row>
     <row r="536" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>942</v>
+        <v>936</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C536" s="0" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="D536" s="1" t="n">
         <v>3.69E-006</v>
@@ -22022,13 +22000,13 @@
     </row>
     <row r="537" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>943</v>
+        <v>937</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C537" s="0" t="s">
-        <v>944</v>
+        <v>938</v>
       </c>
       <c r="D537" s="1" t="n">
         <v>2.2E-006</v>
@@ -22057,13 +22035,13 @@
     </row>
     <row r="538" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="0" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="B538" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C538" s="0" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="D538" s="1" t="n">
         <v>1.3E-005</v>
@@ -22092,13 +22070,13 @@
     </row>
     <row r="539" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="0" t="s">
-        <v>945</v>
+        <v>939</v>
       </c>
       <c r="B539" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C539" s="0" t="s">
-        <v>946</v>
+        <v>940</v>
       </c>
       <c r="D539" s="0" t="n">
         <v>0.00041</v>
@@ -22127,13 +22105,13 @@
     </row>
     <row r="540" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="0" t="s">
-        <v>947</v>
+        <v>941</v>
       </c>
       <c r="B540" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C540" s="0" t="s">
-        <v>948</v>
+        <v>942</v>
       </c>
       <c r="D540" s="0" t="n">
         <v>0.00037</v>
@@ -22162,13 +22140,13 @@
     </row>
     <row r="541" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="0" t="s">
-        <v>902</v>
+        <v>896</v>
       </c>
       <c r="B541" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C541" s="0" t="s">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="D541" s="0" t="n">
         <v>0.00087</v>
@@ -22232,13 +22210,13 @@
     </row>
     <row r="543" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="0" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="B543" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C543" s="0" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="D543" s="1" t="n">
         <v>1.69E-005</v>
@@ -22267,13 +22245,13 @@
     </row>
     <row r="544" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="0" t="s">
-        <v>949</v>
+        <v>943</v>
       </c>
       <c r="B544" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C544" s="0" t="s">
-        <v>950</v>
+        <v>944</v>
       </c>
       <c r="D544" s="1" t="n">
         <v>3.9E-005</v>
@@ -22302,13 +22280,13 @@
     </row>
     <row r="545" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A545" s="0" t="s">
-        <v>951</v>
+        <v>945</v>
       </c>
       <c r="B545" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C545" s="0" t="s">
-        <v>952</v>
+        <v>946</v>
       </c>
       <c r="D545" s="0" t="n">
         <v>0.00021</v>
@@ -22337,13 +22315,13 @@
     </row>
     <row r="546" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A546" s="0" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="B546" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C546" s="0" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="D546" s="0" t="n">
         <v>0.000188</v>
@@ -22372,13 +22350,13 @@
     </row>
     <row r="547" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A547" s="0" t="s">
-        <v>955</v>
+        <v>949</v>
       </c>
       <c r="B547" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C547" s="0" t="s">
-        <v>956</v>
+        <v>950</v>
       </c>
       <c r="D547" s="1" t="n">
         <v>6.39E-005</v>
@@ -22407,13 +22385,13 @@
     </row>
     <row r="548" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A548" s="0" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
       <c r="B548" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C548" s="0" t="s">
-        <v>958</v>
+        <v>952</v>
       </c>
       <c r="D548" s="1" t="n">
         <v>6.74E-005</v>
@@ -22442,13 +22420,13 @@
     </row>
     <row r="549" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A549" s="0" t="s">
-        <v>959</v>
+        <v>953</v>
       </c>
       <c r="B549" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C549" s="0" t="s">
-        <v>960</v>
+        <v>954</v>
       </c>
       <c r="D549" s="1" t="n">
         <v>9.18E-005</v>
@@ -22477,13 +22455,13 @@
     </row>
     <row r="550" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A550" s="0" t="s">
-        <v>961</v>
+        <v>955</v>
       </c>
       <c r="B550" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C550" s="0" t="s">
-        <v>962</v>
+        <v>956</v>
       </c>
       <c r="D550" s="0" t="n">
         <v>0.000343</v>
@@ -22512,13 +22490,13 @@
     </row>
     <row r="551" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="0" t="s">
-        <v>963</v>
+        <v>957</v>
       </c>
       <c r="B551" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C551" s="0" t="s">
-        <v>964</v>
+        <v>958</v>
       </c>
       <c r="D551" s="1" t="n">
         <v>7.1E-006</v>
@@ -22547,13 +22525,13 @@
     </row>
     <row r="552" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A552" s="0" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="B552" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C552" s="0" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="D552" s="1" t="n">
         <v>5.4E-006</v>
@@ -22582,13 +22560,13 @@
     </row>
     <row r="553" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="0" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="B553" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C553" s="0" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="D553" s="1" t="n">
         <v>1.5E-005</v>
@@ -22617,13 +22595,13 @@
     </row>
     <row r="554" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="0" t="s">
-        <v>943</v>
+        <v>937</v>
       </c>
       <c r="B554" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C554" s="0" t="s">
-        <v>944</v>
+        <v>938</v>
       </c>
       <c r="D554" s="1" t="n">
         <v>2.2E-006</v>
@@ -22652,13 +22630,13 @@
     </row>
     <row r="555" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A555" s="0" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="B555" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C555" s="0" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="D555" s="1" t="n">
         <v>4E-005</v>
@@ -22687,13 +22665,13 @@
     </row>
     <row r="556" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A556" s="0" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="B556" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C556" s="0" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="D556" s="1" t="n">
         <v>7E-006</v>
@@ -22722,13 +22700,13 @@
     </row>
     <row r="557" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A557" s="0" t="s">
-        <v>965</v>
+        <v>959</v>
       </c>
       <c r="B557" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C557" s="0" t="s">
-        <v>966</v>
+        <v>960</v>
       </c>
       <c r="D557" s="0" t="n">
         <v>0.000903</v>
@@ -22757,13 +22735,13 @@
     </row>
     <row r="558" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A558" s="0" t="s">
-        <v>967</v>
+        <v>961</v>
       </c>
       <c r="B558" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C558" s="0" t="s">
-        <v>968</v>
+        <v>962</v>
       </c>
       <c r="D558" s="0" t="n">
         <v>0.000103</v>
@@ -22792,13 +22770,13 @@
     </row>
     <row r="559" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A559" s="0" t="s">
-        <v>969</v>
+        <v>963</v>
       </c>
       <c r="B559" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C559" s="0" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="D559" s="0" t="n">
         <v>0.000254</v>
@@ -22827,13 +22805,13 @@
     </row>
     <row r="560" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A560" s="0" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="B560" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C560" s="0" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
       <c r="D560" s="0" t="n">
         <v>0.000614</v>
@@ -22862,13 +22840,13 @@
     </row>
     <row r="561" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="0" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="B561" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C561" s="0" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="D561" s="1" t="n">
         <v>1.59E-005</v>
@@ -22897,13 +22875,13 @@
     </row>
     <row r="562" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A562" s="0" t="s">
-        <v>973</v>
+        <v>967</v>
       </c>
       <c r="B562" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C562" s="0" t="s">
-        <v>974</v>
+        <v>968</v>
       </c>
       <c r="D562" s="1" t="n">
         <v>7.11E-006</v>
@@ -22932,13 +22910,13 @@
     </row>
     <row r="563" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A563" s="0" t="s">
-        <v>975</v>
+        <v>969</v>
       </c>
       <c r="B563" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C563" s="0" t="s">
-        <v>976</v>
+        <v>970</v>
       </c>
       <c r="D563" s="1" t="n">
         <v>5.17E-006</v>
@@ -22967,13 +22945,13 @@
     </row>
     <row r="564" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A564" s="0" t="s">
-        <v>977</v>
+        <v>971</v>
       </c>
       <c r="B564" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C564" s="0" t="s">
-        <v>978</v>
+        <v>972</v>
       </c>
       <c r="D564" s="1" t="n">
         <v>2.15E-005</v>
@@ -23002,13 +22980,13 @@
     </row>
     <row r="565" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A565" s="0" t="s">
-        <v>979</v>
+        <v>973</v>
       </c>
       <c r="B565" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C565" s="0" t="s">
-        <v>980</v>
+        <v>974</v>
       </c>
       <c r="D565" s="1" t="n">
         <v>1.18E-005</v>
@@ -23037,13 +23015,13 @@
     </row>
     <row r="566" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A566" s="0" t="s">
-        <v>981</v>
+        <v>975</v>
       </c>
       <c r="B566" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C566" s="0" t="s">
-        <v>982</v>
+        <v>976</v>
       </c>
       <c r="D566" s="1" t="n">
         <v>1.4E-005</v>
@@ -23107,13 +23085,13 @@
     </row>
     <row r="568" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A568" s="0" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="B568" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C568" s="0" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="D568" s="0" t="n">
         <v>0.000532</v>
@@ -23142,13 +23120,13 @@
     </row>
     <row r="569" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A569" s="0" t="s">
-        <v>983</v>
+        <v>977</v>
       </c>
       <c r="B569" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C569" s="0" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
       <c r="D569" s="1" t="n">
         <v>1.34E-005</v>
@@ -23177,13 +23155,13 @@
     </row>
     <row r="570" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A570" s="0" t="s">
-        <v>985</v>
+        <v>979</v>
       </c>
       <c r="B570" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C570" s="0" t="s">
-        <v>986</v>
+        <v>980</v>
       </c>
       <c r="D570" s="1" t="n">
         <v>1.44E-005</v>
@@ -23212,13 +23190,13 @@
     </row>
     <row r="571" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A571" s="0" t="s">
-        <v>987</v>
+        <v>981</v>
       </c>
       <c r="B571" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C571" s="0" t="s">
-        <v>988</v>
+        <v>982</v>
       </c>
       <c r="D571" s="1" t="n">
         <v>5.71E-006</v>
@@ -23247,13 +23225,13 @@
     </row>
     <row r="572" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A572" s="0" t="s">
-        <v>989</v>
+        <v>983</v>
       </c>
       <c r="B572" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C572" s="0" t="s">
-        <v>990</v>
+        <v>984</v>
       </c>
       <c r="D572" s="1" t="n">
         <v>9.13E-006</v>
@@ -23282,13 +23260,13 @@
     </row>
     <row r="573" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A573" s="0" t="s">
-        <v>991</v>
+        <v>985</v>
       </c>
       <c r="B573" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C573" s="0" t="s">
-        <v>992</v>
+        <v>986</v>
       </c>
       <c r="D573" s="1" t="n">
         <v>9.68E-006</v>
@@ -23317,13 +23295,13 @@
     </row>
     <row r="574" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A574" s="0" t="s">
-        <v>993</v>
+        <v>987</v>
       </c>
       <c r="B574" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C574" s="0" t="s">
-        <v>994</v>
+        <v>988</v>
       </c>
       <c r="D574" s="0" t="n">
         <v>0.0001</v>
@@ -23352,13 +23330,13 @@
     </row>
     <row r="575" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A575" s="0" t="s">
-        <v>995</v>
+        <v>989</v>
       </c>
       <c r="B575" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C575" s="0" t="s">
-        <v>996</v>
+        <v>990</v>
       </c>
       <c r="D575" s="1" t="n">
         <v>5.9E-005</v>
@@ -23387,13 +23365,13 @@
     </row>
     <row r="576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A576" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="B576" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C576" s="0" t="s">
-        <v>998</v>
+        <v>992</v>
       </c>
       <c r="D576" s="0" t="n">
         <v>0.00077</v>
@@ -23422,13 +23400,13 @@
     </row>
     <row r="577" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A577" s="0" t="s">
-        <v>999</v>
+        <v>993</v>
       </c>
       <c r="B577" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C577" s="0" t="s">
-        <v>1000</v>
+        <v>994</v>
       </c>
       <c r="D577" s="0" t="n">
         <v>0.00066</v>
@@ -23457,13 +23435,13 @@
     </row>
     <row r="578" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A578" s="0" t="s">
-        <v>1001</v>
+        <v>995</v>
       </c>
       <c r="B578" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C578" s="0" t="s">
-        <v>1002</v>
+        <v>996</v>
       </c>
       <c r="D578" s="0" t="n">
         <v>0.00045</v>
@@ -23492,13 +23470,13 @@
     </row>
     <row r="579" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A579" s="0" t="s">
-        <v>1003</v>
+        <v>997</v>
       </c>
       <c r="B579" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C579" s="0" t="s">
-        <v>1004</v>
+        <v>998</v>
       </c>
       <c r="D579" s="0" t="n">
         <v>0.00026</v>
@@ -23527,13 +23505,13 @@
     </row>
     <row r="580" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A580" s="0" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="B580" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C580" s="0" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="D580" s="0" t="s">
         <v>25</v>
@@ -23597,13 +23575,13 @@
     </row>
     <row r="582" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A582" s="0" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="B582" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C582" s="0" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="D582" s="0" t="n">
         <v>0.000313</v>
@@ -23632,13 +23610,13 @@
     </row>
     <row r="583" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A583" s="0" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
       <c r="B583" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C583" s="0" t="s">
-        <v>1008</v>
+        <v>1002</v>
       </c>
       <c r="D583" s="0" t="n">
         <v>0.000317</v>
@@ -23667,13 +23645,13 @@
     </row>
     <row r="584" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A584" s="0" t="s">
-        <v>1009</v>
+        <v>1003</v>
       </c>
       <c r="B584" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C584" s="0" t="s">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="D584" s="0" t="n">
         <v>0.000436</v>
@@ -23702,13 +23680,13 @@
     </row>
     <row r="585" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A585" s="0" t="s">
-        <v>1011</v>
+        <v>1005</v>
       </c>
       <c r="B585" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C585" s="0" t="s">
-        <v>1012</v>
+        <v>1006</v>
       </c>
       <c r="D585" s="0" t="n">
         <v>0.000226</v>
@@ -23772,13 +23750,13 @@
     </row>
     <row r="587" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A587" s="0" t="s">
-        <v>1013</v>
+        <v>1007</v>
       </c>
       <c r="B587" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C587" s="0" t="s">
-        <v>1014</v>
+        <v>1008</v>
       </c>
       <c r="D587" s="0" t="n">
         <v>0.00031</v>
@@ -23807,13 +23785,13 @@
     </row>
     <row r="588" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A588" s="0" t="s">
-        <v>1015</v>
+        <v>1009</v>
       </c>
       <c r="B588" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C588" s="0" t="s">
-        <v>1016</v>
+        <v>1010</v>
       </c>
       <c r="D588" s="0" t="n">
         <v>0.000956</v>
@@ -23842,13 +23820,13 @@
     </row>
     <row r="589" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="0" t="s">
-        <v>1017</v>
+        <v>1011</v>
       </c>
       <c r="B589" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C589" s="0" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="D589" s="1" t="n">
         <v>1.3E-005</v>
@@ -23877,13 +23855,13 @@
     </row>
     <row r="590" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A590" s="0" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="B590" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C590" s="0" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="D590" s="1" t="n">
         <v>1.54E-006</v>
@@ -23912,13 +23890,13 @@
     </row>
     <row r="591" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A591" s="0" t="s">
-        <v>928</v>
+        <v>922</v>
       </c>
       <c r="B591" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C591" s="0" t="s">
-        <v>929</v>
+        <v>923</v>
       </c>
       <c r="D591" s="1" t="n">
         <v>2.2E-005</v>
@@ -23947,13 +23925,13 @@
     </row>
     <row r="592" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A592" s="0" t="s">
-        <v>1018</v>
+        <v>1012</v>
       </c>
       <c r="B592" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C592" s="0" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
       <c r="D592" s="0" t="n">
         <v>0.0008</v>
@@ -23982,13 +23960,13 @@
     </row>
     <row r="593" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A593" s="0" t="s">
-        <v>888</v>
+        <v>882</v>
       </c>
       <c r="B593" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C593" s="0" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="D593" s="0" t="n">
         <v>0.00035</v>
@@ -24017,13 +23995,13 @@
     </row>
     <row r="594" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A594" s="0" t="s">
-        <v>1020</v>
+        <v>1014</v>
       </c>
       <c r="B594" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C594" s="0" t="s">
-        <v>962</v>
+        <v>956</v>
       </c>
       <c r="D594" s="0" t="n">
         <v>0.00027</v>
@@ -24052,13 +24030,13 @@
     </row>
     <row r="595" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A595" s="0" t="s">
-        <v>1021</v>
+        <v>1015</v>
       </c>
       <c r="B595" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C595" s="0" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="D595" s="0" t="n">
         <v>0.00092</v>
@@ -24087,13 +24065,13 @@
     </row>
     <row r="596" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A596" s="0" t="s">
-        <v>1022</v>
+        <v>1016</v>
       </c>
       <c r="B596" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C596" s="0" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="D596" s="0" t="n">
         <v>0.00073</v>
@@ -24122,13 +24100,13 @@
     </row>
     <row r="597" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A597" s="0" t="s">
-        <v>1023</v>
+        <v>1017</v>
       </c>
       <c r="B597" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C597" s="0" t="s">
-        <v>899</v>
+        <v>893</v>
       </c>
       <c r="D597" s="0" t="n">
         <v>0.00032</v>
@@ -24157,13 +24135,13 @@
     </row>
     <row r="598" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A598" s="0" t="s">
-        <v>1024</v>
+        <v>1018</v>
       </c>
       <c r="B598" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C598" s="0" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="D598" s="0" t="n">
         <v>0.00028</v>
@@ -24192,13 +24170,13 @@
     </row>
     <row r="599" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A599" s="0" t="s">
-        <v>1025</v>
+        <v>1019</v>
       </c>
       <c r="B599" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C599" s="0" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="D599" s="0" t="n">
         <v>0.00016</v>
@@ -24227,13 +24205,13 @@
     </row>
     <row r="600" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A600" s="0" t="s">
-        <v>1026</v>
+        <v>1020</v>
       </c>
       <c r="B600" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C600" s="0" t="s">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="D600" s="0" t="n">
         <v>0.00063</v>
@@ -24262,13 +24240,13 @@
     </row>
     <row r="601" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A601" s="0" t="s">
-        <v>1027</v>
+        <v>1021</v>
       </c>
       <c r="B601" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C601" s="0" t="s">
-        <v>1028</v>
+        <v>1022</v>
       </c>
       <c r="D601" s="1" t="n">
         <v>2.51E-005</v>
@@ -24297,13 +24275,13 @@
     </row>
     <row r="602" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A602" s="0" t="s">
-        <v>1029</v>
+        <v>1023</v>
       </c>
       <c r="B602" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C602" s="0" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="D602" s="1" t="n">
         <v>2.11E-006</v>
@@ -24332,13 +24310,13 @@
     </row>
     <row r="603" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A603" s="0" t="s">
-        <v>936</v>
+        <v>930</v>
       </c>
       <c r="B603" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C603" s="0" t="s">
-        <v>937</v>
+        <v>931</v>
       </c>
       <c r="D603" s="1" t="n">
         <v>2.06E-006</v>
@@ -24367,13 +24345,13 @@
     </row>
     <row r="604" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A604" s="0" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="B604" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C604" s="0" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="D604" s="0" t="n">
         <v>0.000794</v>
@@ -24402,13 +24380,13 @@
     </row>
     <row r="605" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A605" s="0" t="s">
-        <v>1030</v>
+        <v>1024</v>
       </c>
       <c r="B605" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C605" s="0" t="s">
-        <v>1031</v>
+        <v>1025</v>
       </c>
       <c r="D605" s="0" t="n">
         <v>0.000832</v>
@@ -24437,13 +24415,13 @@
     </row>
     <row r="606" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A606" s="0" t="s">
-        <v>1032</v>
+        <v>1026</v>
       </c>
       <c r="B606" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C606" s="0" t="s">
-        <v>1033</v>
+        <v>1027</v>
       </c>
       <c r="D606" s="0" t="n">
         <v>0.000834</v>
@@ -24472,13 +24450,13 @@
     </row>
     <row r="607" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A607" s="0" t="s">
-        <v>1034</v>
+        <v>1028</v>
       </c>
       <c r="B607" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C607" s="0" t="s">
-        <v>1035</v>
+        <v>1029</v>
       </c>
       <c r="D607" s="0" t="n">
         <v>0.000631</v>
@@ -24507,13 +24485,13 @@
     </row>
     <row r="608" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A608" s="0" t="s">
-        <v>1036</v>
+        <v>1030</v>
       </c>
       <c r="B608" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C608" s="0" t="s">
-        <v>1037</v>
+        <v>1031</v>
       </c>
       <c r="D608" s="0" t="n">
         <v>0.000492</v>
@@ -24542,13 +24520,13 @@
     </row>
     <row r="609" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A609" s="0" t="s">
-        <v>1038</v>
+        <v>1032</v>
       </c>
       <c r="B609" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C609" s="0" t="s">
-        <v>1039</v>
+        <v>1033</v>
       </c>
       <c r="D609" s="1" t="n">
         <v>2.65E-006</v>

</xml_diff>